<commit_message>
Added comments on the FIN684F_Project_III.py file and checked final outputs.
</commit_message>
<xml_diff>
--- a/analysis_report_CAPM_FF3F_196301_199312.xlsx
+++ b/analysis_report_CAPM_FF3F_196301_199312.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Main Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Regression Outputs" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Covariance Matrices" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="GRS Test Outputs" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="FMB Outputs" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Charts" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Regression Outputs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Covariance Matrices" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GRS Test Outputs" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FMB Outputs" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Charts" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -160,13 +160,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -185,13 +185,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -210,13 +210,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -235,13 +235,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -260,13 +260,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>

</xml_diff>

<commit_message>
Added conclusion on whether or not to reject null hypothesis.
</commit_message>
<xml_diff>
--- a/analysis_report_CAPM_FF3F_196301_199312.xlsx
+++ b/analysis_report_CAPM_FF3F_196301_199312.xlsx
@@ -1173,10 +1173,15 @@
       </c>
       <c r="E39" s="2" t="inlineStr">
         <is>
+          <t>Conclusion</t>
+        </is>
+      </c>
+      <c r="F39" s="2" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F39" s="2" t="inlineStr">
+      <c r="G39" s="2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1200,10 +1205,15 @@
       <c r="D41" s="3" t="n">
         <v>1.184748583016315e-05</v>
       </c>
-      <c r="E41" s="3" t="n">
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t>Reject Null</t>
+        </is>
+      </c>
+      <c r="F41" s="3" t="n">
         <v>372</v>
       </c>
-      <c r="F41" s="3" t="n">
+      <c r="G41" s="3" t="n">
         <v>25</v>
       </c>
     </row>
@@ -1348,10 +1358,15 @@
       </c>
       <c r="E52" s="2" t="inlineStr">
         <is>
+          <t>Conclusion</t>
+        </is>
+      </c>
+      <c r="F52" s="2" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F52" s="2" t="inlineStr">
+      <c r="G52" s="2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -1375,10 +1390,15 @@
       <c r="D54" s="3" t="n">
         <v>0.003736014601147697</v>
       </c>
-      <c r="E54" s="3" t="n">
+      <c r="E54" s="3" t="inlineStr">
+        <is>
+          <t>Reject Null</t>
+        </is>
+      </c>
+      <c r="F54" s="3" t="n">
         <v>372</v>
       </c>
-      <c r="F54" s="3" t="n">
+      <c r="G54" s="3" t="n">
         <v>25</v>
       </c>
     </row>
@@ -9188,7 +9208,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9243,10 +9263,15 @@
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
+          <t>Conclusion</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F3" s="2" t="inlineStr">
+      <c r="G3" s="2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -9270,10 +9295,15 @@
       <c r="D5" s="3" t="n">
         <v>1.184748583016315e-05</v>
       </c>
-      <c r="E5" s="3" t="n">
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Reject Null</t>
+        </is>
+      </c>
+      <c r="F5" s="3" t="n">
         <v>372</v>
       </c>
-      <c r="F5" s="3" t="n">
+      <c r="G5" s="3" t="n">
         <v>25</v>
       </c>
     </row>
@@ -9303,10 +9333,15 @@
       </c>
       <c r="E9" s="2" t="inlineStr">
         <is>
+          <t>Conclusion</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
           <t>T</t>
         </is>
       </c>
-      <c r="F9" s="2" t="inlineStr">
+      <c r="G9" s="2" t="inlineStr">
         <is>
           <t>N</t>
         </is>
@@ -9330,10 +9365,15 @@
       <c r="D11" s="3" t="n">
         <v>0.003736014601147697</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="3" t="inlineStr">
+        <is>
+          <t>Reject Null</t>
+        </is>
+      </c>
+      <c r="F11" s="3" t="n">
         <v>372</v>
       </c>
-      <c r="F11" s="3" t="n">
+      <c r="G11" s="3" t="n">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Casted start and end dates in the FIN684F_Project_III.ipynb file for the code to properly work.
</commit_message>
<xml_diff>
--- a/analysis_report_CAPM_FF3F_196301_199312.xlsx
+++ b/analysis_report_CAPM_FF3F_196301_199312.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Regression Outputs" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Covariance Matrices" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GRS Test Outputs" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FMB Outputs" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Charts" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Main Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Regression Outputs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Covariance Matrices" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="GRS Test Outputs" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="FMB Outputs" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Charts" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -160,13 +160,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId1"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -185,13 +185,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId2"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -210,13 +210,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId3"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -235,13 +235,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId4"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -260,13 +260,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
-        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+        <a:blip cstate="print" r:embed="rId5"/>
+        <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+        <a:prstGeom prst="rect"/>
       </spPr>
     </pic>
     <clientData/>

</xml_diff>

<commit_message>
Changed formatting for start date and end date in output excel file.
</commit_message>
<xml_diff>
--- a/analysis_report_CAPM_FF3F_196301_199312.xlsx
+++ b/analysis_report_CAPM_FF3F_196301_199312.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Main Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Regression Outputs" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Covariance Matrices" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="GRS Test Outputs" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="FMB Outputs" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Charts" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Main Summary" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Portfolio Summary" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Regression Outputs" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Covariance Matrices" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="GRS Test Outputs" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FMB Outputs" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Charts" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>0</col>
@@ -160,13 +160,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId1"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -185,13 +185,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId2"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId2"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -210,13 +210,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId3"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId3"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -235,13 +235,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId4"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId4"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -260,13 +260,13 @@
         <cNvPicPr/>
       </nvPicPr>
       <blipFill>
-        <a:blip cstate="print" r:embed="rId5"/>
-        <a:stretch>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId5"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
       </blipFill>
       <spPr>
-        <a:prstGeom prst="rect"/>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
       </spPr>
     </pic>
     <clientData/>
@@ -619,7 +619,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>1963-01-31 00:00:00</t>
+          <t>1963-01</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>1993-12-31 00:00:00</t>
+          <t>1993-12</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed excel output columns names from Beta_MKT to Lambda_MKT.
</commit_message>
<xml_diff>
--- a/analysis_report_CAPM_FF3F_196301_199312.xlsx
+++ b/analysis_report_CAPM_FF3F_196301_199312.xlsx
@@ -1273,7 +1273,7 @@
     <row r="47">
       <c r="A47" s="3" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Lambda_Alpha</t>
         </is>
       </c>
       <c r="B47" s="3" t="n">
@@ -1304,7 +1304,7 @@
     <row r="48">
       <c r="A48" s="3" t="inlineStr">
         <is>
-          <t>Beta_MKT</t>
+          <t>Lambda_MKT</t>
         </is>
       </c>
       <c r="B48" s="3" t="n">
@@ -1458,7 +1458,7 @@
     <row r="60">
       <c r="A60" s="3" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Lambda_Alpha</t>
         </is>
       </c>
       <c r="B60" s="3" t="n">
@@ -1489,7 +1489,7 @@
     <row r="61">
       <c r="A61" s="3" t="inlineStr">
         <is>
-          <t>Beta_MKT</t>
+          <t>Lambda_MKT</t>
         </is>
       </c>
       <c r="B61" s="3" t="n">
@@ -1520,7 +1520,7 @@
     <row r="62">
       <c r="A62" s="3" t="inlineStr">
         <is>
-          <t>Beta_SMB</t>
+          <t>Lambda_SMB</t>
         </is>
       </c>
       <c r="B62" s="3" t="n">
@@ -1551,7 +1551,7 @@
     <row r="63">
       <c r="A63" s="3" t="inlineStr">
         <is>
-          <t>Beta_HML</t>
+          <t>Lambda_HML</t>
         </is>
       </c>
       <c r="B63" s="3" t="n">
@@ -9473,7 +9473,7 @@
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Lambda_Alpha</t>
         </is>
       </c>
       <c r="B5" s="3" t="n">
@@ -9504,7 +9504,7 @@
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
         <is>
-          <t>Beta_MKT</t>
+          <t>Lambda_MKT</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
@@ -9588,7 +9588,7 @@
     <row r="12">
       <c r="A12" s="3" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Lambda_Alpha</t>
         </is>
       </c>
       <c r="B12" s="3" t="n">
@@ -9619,7 +9619,7 @@
     <row r="13">
       <c r="A13" s="3" t="inlineStr">
         <is>
-          <t>Beta_MKT</t>
+          <t>Lambda_MKT</t>
         </is>
       </c>
       <c r="B13" s="3" t="n">
@@ -9650,7 +9650,7 @@
     <row r="14">
       <c r="A14" s="3" t="inlineStr">
         <is>
-          <t>Beta_SMB</t>
+          <t>Lambda_SMB</t>
         </is>
       </c>
       <c r="B14" s="3" t="n">
@@ -9681,7 +9681,7 @@
     <row r="15">
       <c r="A15" s="3" t="inlineStr">
         <is>
-          <t>Beta_HML</t>
+          <t>Lambda_HML</t>
         </is>
       </c>
       <c r="B15" s="3" t="n">

</xml_diff>